<commit_message>
Hopefully finished and correct
</commit_message>
<xml_diff>
--- a/BOM template.xlsx
+++ b/BOM template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sienna\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sienna\Documents\KinetisWorkSpace\CC2511_AssignmentGroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="19140" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="19140" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Group number:</t>
   </si>
@@ -71,9 +71,6 @@
     <t>5V regulator</t>
   </si>
   <si>
-    <t>(example only; delete if not needed)</t>
-  </si>
-  <si>
     <t>Components are subject to approval from the subject coordinator. Expensive orders may be declined.</t>
   </si>
   <si>
@@ -105,6 +102,39 @@
   </si>
   <si>
     <t>Sienna-Rose Price</t>
+  </si>
+  <si>
+    <t>Fixed, 10V -35V In; 5V And 1.5A Out</t>
+  </si>
+  <si>
+    <t>Logic Chip</t>
+  </si>
+  <si>
+    <t>Quad, 2-input Nor Gate; SN74HC02N</t>
+  </si>
+  <si>
+    <t>P-Type Power MOSFET</t>
+  </si>
+  <si>
+    <t>N-Type Power MOSFET</t>
+  </si>
+  <si>
+    <t>16.5 A, -100 V, 190 mohm, -10 V, -4 V</t>
+  </si>
+  <si>
+    <t>22 A, 30 V, 45 mohm, 10 V, 1 V</t>
+  </si>
+  <si>
+    <t>8-Pin Header</t>
+  </si>
+  <si>
+    <t>Single Row, 8 Pin Female Headers</t>
+  </si>
+  <si>
+    <t>2-Pin Header</t>
+  </si>
+  <si>
+    <t>Single Row, 2 Pin Male Header</t>
   </si>
 </sst>
 </file>
@@ -115,7 +145,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +172,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -357,6 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -640,15 +678,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="48" customWidth="1"/>
@@ -656,7 +694,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -684,7 +722,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -704,7 +742,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -714,7 +752,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -742,7 +780,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -793,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="4"/>
@@ -803,7 +841,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="4"/>
@@ -813,7 +851,7 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="4"/>
@@ -879,41 +917,64 @@
         <v>1.54</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="25"/>
+      <c r="A24" s="26">
+        <v>9590919</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="25">
+        <v>0.76</v>
+      </c>
       <c r="E24" s="25">
-        <f t="shared" ref="E24:E42" si="0">D24*B24</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="2"/>
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="2"/>
+      <c r="A25" s="2">
+        <v>8660239</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="25">
+        <v>1.74</v>
+      </c>
+      <c r="E25" s="25"/>
+      <c r="F25" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="2"/>
+      <c r="A26" s="2">
+        <v>9846514</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="25">
+        <v>1.58</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
@@ -921,7 +982,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="25"/>
       <c r="E27" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E24:E42" si="0">D27*B27</f>
         <v>0</v>
       </c>
       <c r="F27" s="2"/>
@@ -1100,18 +1161,18 @@
       <c r="D43" s="18"/>
       <c r="E43" s="19">
         <f>SUM(E23:E42)</f>
-        <v>1.54</v>
+        <v>2.2960000000000003</v>
       </c>
       <c r="F43" s="16"/>
     </row>
     <row r="46" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>9</v>
@@ -1126,13 +1187,19 @@
         <v>12</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
+      <c r="A48" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="14">
+        <v>3</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>34</v>
+      </c>
       <c r="D48" s="24"/>
       <c r="E48" s="24">
         <f>D48*B48</f>
@@ -1141,9 +1208,15 @@
       <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
+      <c r="A49" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="14">
+        <v>1</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="D49" s="24"/>
       <c r="E49" s="24">
         <f t="shared" ref="E49:E56" si="1">D49*B49</f>

</xml_diff>

<commit_message>
Finished sch. will update BOM
</commit_message>
<xml_diff>
--- a/BOM template.xlsx
+++ b/BOM template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sienna\Documents\KinetisWorkSpace\CC2511_AssignmentGroup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jc240979\Desktop\CC2511_AssignmentGroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Group number:</t>
   </si>
@@ -135,15 +135,33 @@
   </si>
   <si>
     <t>Single Row, 2 Pin Male Header</t>
+  </si>
+  <si>
+    <t>Diode 1A 50V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1N4001 </t>
+  </si>
+  <si>
+    <t>4k7 Resistor</t>
+  </si>
+  <si>
+    <t>0.33uF Capacitor</t>
+  </si>
+  <si>
+    <t>0.1 uF Capacitor</t>
+  </si>
+  <si>
+    <t>1uF Capacitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -365,7 +383,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -387,13 +405,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -678,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +963,7 @@
         <v>8660239</v>
       </c>
       <c r="B25" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>30</v>
@@ -953,7 +971,10 @@
       <c r="D25" s="25">
         <v>1.74</v>
       </c>
-      <c r="E25" s="25"/>
+      <c r="E25" s="25">
+        <f xml:space="preserve"> B25*D25</f>
+        <v>8.6999999999999993</v>
+      </c>
       <c r="F25" s="2" t="s">
         <v>32</v>
       </c>
@@ -971,7 +992,10 @@
       <c r="D26" s="25">
         <v>1.58</v>
       </c>
-      <c r="E26" s="25"/>
+      <c r="E26" s="25">
+        <f>B26*D26</f>
+        <v>3.16</v>
+      </c>
       <c r="F26" s="2" t="s">
         <v>31</v>
       </c>
@@ -982,7 +1006,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="25"/>
       <c r="E27" s="25">
-        <f t="shared" ref="E24:E42" si="0">D27*B27</f>
+        <f t="shared" ref="E27:E42" si="0">D27*B27</f>
         <v>0</v>
       </c>
       <c r="F27" s="2"/>
@@ -1161,7 +1185,7 @@
       <c r="D43" s="18"/>
       <c r="E43" s="19">
         <f>SUM(E23:E42)</f>
-        <v>2.2960000000000003</v>
+        <v>14.155999999999999</v>
       </c>
       <c r="F43" s="16"/>
     </row>
@@ -1225,9 +1249,15 @@
       <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
+      <c r="A50" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="14">
+        <v>2</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="D50" s="24"/>
       <c r="E50" s="24">
         <f t="shared" si="1"/>
@@ -1237,8 +1267,12 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
+      <c r="B51" s="14">
+        <v>2</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="D51" s="24"/>
       <c r="E51" s="24">
         <f t="shared" si="1"/>
@@ -1248,8 +1282,12 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
+      <c r="B52" s="14">
+        <v>1</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="D52" s="24"/>
       <c r="E52" s="24">
         <f t="shared" si="1"/>
@@ -1259,8 +1297,12 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
+      <c r="B53" s="14">
+        <v>1</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>41</v>
+      </c>
       <c r="D53" s="24"/>
       <c r="E53" s="24">
         <f t="shared" si="1"/>
@@ -1270,8 +1312,12 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
+      <c r="B54" s="14">
+        <v>1</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="D54" s="24"/>
       <c r="E54" s="24">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Updated as per Mostifa's comments
</commit_message>
<xml_diff>
--- a/BOM template.xlsx
+++ b/BOM template.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jc240979\Desktop\CC2511_AssignmentGroup\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="900" windowWidth="19140" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Group number:</t>
   </si>
@@ -128,15 +123,9 @@
     <t>8-Pin Header</t>
   </si>
   <si>
-    <t>Single Row, 8 Pin Female Headers</t>
-  </si>
-  <si>
     <t>2-Pin Header</t>
   </si>
   <si>
-    <t>Single Row, 2 Pin Male Header</t>
-  </si>
-  <si>
     <t>Diode 1A 50V</t>
   </si>
   <si>
@@ -153,6 +142,27 @@
   </si>
   <si>
     <t>1uF Capacitor</t>
+  </si>
+  <si>
+    <t>N-Type low current MOSFET</t>
+  </si>
+  <si>
+    <t>200mA, 60V</t>
+  </si>
+  <si>
+    <t>100 ohm Resister</t>
+  </si>
+  <si>
+    <t>Single Row, 8 Pin male Headers</t>
+  </si>
+  <si>
+    <t>Single Row, 2 Pin male Header</t>
+  </si>
+  <si>
+    <t>30 pin, double row header</t>
+  </si>
+  <si>
+    <t>42 pin, double row header</t>
   </si>
 </sst>
 </file>
@@ -686,7 +696,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -696,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +973,7 @@
         <v>8660239</v>
       </c>
       <c r="B25" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>30</v>
@@ -973,7 +983,7 @@
       </c>
       <c r="E25" s="25">
         <f xml:space="preserve"> B25*D25</f>
-        <v>8.6999999999999993</v>
+        <v>5.22</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>32</v>
@@ -1001,15 +1011,25 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="25"/>
+      <c r="A27" s="2">
+        <v>9845178</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="25">
+        <v>0.625</v>
+      </c>
       <c r="E27" s="25">
         <f t="shared" ref="E27:E42" si="0">D27*B27</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="2"/>
+        <v>1.25</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -1185,7 +1205,7 @@
       <c r="D43" s="18"/>
       <c r="E43" s="19">
         <f>SUM(E23:E42)</f>
-        <v>14.155999999999999</v>
+        <v>11.926</v>
       </c>
       <c r="F43" s="16"/>
     </row>
@@ -1222,7 +1242,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="24">
@@ -1233,13 +1253,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B49" s="14">
         <v>1</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="24">
@@ -1250,13 +1270,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B50" s="14">
         <v>2</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="24">
@@ -1271,7 +1291,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D51" s="24"/>
       <c r="E51" s="24">
@@ -1286,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D52" s="24"/>
       <c r="E52" s="24">
@@ -1301,7 +1321,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D53" s="24"/>
       <c r="E53" s="24">
@@ -1316,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D54" s="24"/>
       <c r="E54" s="24">
@@ -1327,8 +1347,12 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
+      <c r="B55" s="14">
+        <v>1</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="D55" s="24"/>
       <c r="E55" s="24">
         <f t="shared" si="1"/>
@@ -1338,8 +1362,12 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
+      <c r="B56" s="14">
+        <v>1</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="D56" s="24"/>
       <c r="E56" s="24">
         <f t="shared" si="1"/>
@@ -1349,8 +1377,12 @@
     </row>
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
+      <c r="B57" s="14">
+        <v>1</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="D57" s="24"/>
       <c r="E57" s="24">
         <f>D57*B57</f>

</xml_diff>